<commit_message>
Updated general results excel
</commit_message>
<xml_diff>
--- a/documentation/user-experience-questionnaires/results/General Results.xlsx
+++ b/documentation/user-experience-questionnaires/results/General Results.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcastro/Faculdade/Mestrado/1-ano/semestre-1/RVA/entrega-2-2021/WebXR-Furniture-Assembly/documentation/user-experience-questionnaires/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670536DA-FE10-BD4B-98B4-7681B3E865D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AAA861-334A-1A49-9521-C6BE17101719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{CF5F6CCD-7D49-FA43-9784-FA6AC14AFB7A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{CF5F6CCD-7D49-FA43-9784-FA6AC14AFB7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Attractiveness</t>
   </si>
@@ -70,6 +70,27 @@
   </si>
   <si>
     <t>Dimension</t>
+  </si>
+  <si>
+    <t>Total CF</t>
+  </si>
+  <si>
+    <t>Total SF</t>
+  </si>
+  <si>
+    <t>Total DF</t>
+  </si>
+  <si>
+    <t>Total RF</t>
+  </si>
+  <si>
+    <t>Total P</t>
+  </si>
+  <si>
+    <t>vr</t>
+  </si>
+  <si>
+    <t>ar</t>
   </si>
 </sst>
 </file>
@@ -131,7 +152,7 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="65" cy="172227"/>
@@ -148,7 +169,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7524750" y="3079750"/>
+          <a:off x="7524750" y="3282950"/>
           <a:ext cx="65" cy="172227"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -482,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BC6C084-2FBD-734A-A130-9985B1E6AB4B}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="A1:E8"/>
+      <selection activeCell="A2" sqref="A2:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,145 +520,274 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.61111111111111105</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="E2" s="1">
-        <f>MEDIAN(B2:D2)</f>
-        <v>0.61111111111111105</v>
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>0.87500000000000011</v>
+        <v>0.61111111111111105</v>
       </c>
       <c r="C3" s="1">
-        <v>0.70833333333333337</v>
+        <v>0.52777777777777779</v>
       </c>
       <c r="D3" s="1">
-        <v>0.79166666666666674</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E8" si="0">MEDIAN(B3:D3)</f>
-        <v>0.79166666666666674</v>
+        <f>MEDIAN(B3:D3)</f>
+        <v>0.61111111111111105</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.87500000000000011</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.79166666666666674</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E9" si="0">MEDIAN(B4:D4)</f>
+        <v>0.79166666666666674</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="1">
         <v>0.875</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D5" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E5" s="1">
         <f t="shared" si="0"/>
         <v>0.875</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>0.375</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>0.375</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D6" s="1">
         <v>0.375</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E6" s="1">
         <f t="shared" si="0"/>
         <v>0.375</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <v>0.20833333333333331</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D7" s="1">
         <v>0.5</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="1">
         <v>0.125</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D8" s="1">
         <v>0.33333333333333337</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E8" s="1">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9" s="1">
         <v>0.55128205128205121</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <v>0.46794871794871795</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D9" s="1">
         <v>0.6217948717948717</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E9" s="1">
         <f t="shared" si="0"/>
         <v>0.55128205128205121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="e">
+        <f>(B21-B27)/(C27-B27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C14" s="1" t="e">
+        <f>(C21-B27)/(C27-B27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D14" s="1" t="e">
+        <f>(D21-B27)/(C27-B27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E14" s="1" t="e">
+        <f>MEDIAN(B14:D14)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="e">
+        <f>(B22-B28)/(C28-B28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C15" s="1" t="e">
+        <f>(C22-B28)/(C28-B28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D15" s="1" t="e">
+        <f t="shared" ref="D15:D18" si="1">(D22-B28)/(C28-B28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E15" s="1" t="e">
+        <f t="shared" ref="E15:E18" si="2">MEDIAN(B15:D15)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="e">
+        <f>(B23-B29)/(C29-B29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C16" s="1" t="e">
+        <f>(C23-B29)/(C29-B29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D16" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E16" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="e">
+        <f>(B24-B30)/(C30-B30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C17" s="1" t="e">
+        <f>(C24-B30)/(C30-B30)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D17" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E17" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="e">
+        <f>(B25-B31)/(C31-B31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C18" s="1" t="e">
+        <f>(C25-B31)/(C31-B31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D18" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E18" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>